<commit_message>
Separated funcionalities from droolsbundle
</commit_message>
<xml_diff>
--- a/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/dtables/dimmer-dtable.xlsx
+++ b/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/dtables/dimmer-dtable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dandrid\smarthome-cep-demonstrator\runtime\com.incquerylabs.smarthome.droolsbundle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dandrid\smarthome-cep-demonstrator\demo\com.incquerylabs.smarthome.demorules.homeio\src\main\resources\dtables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -96,14 +96,6 @@
     <t>Variables</t>
   </si>
   <si>
-    <t>org.eclipse.smarthome.core.items.Item,
-org.eclipse.smarthome.core.library.types.IncreaseDecreaseType,
-org.eclipse.smarthome.core.library.types.OpenClosedType,
-com.incquerylabs.smarthome.droolsbundle.ItemStateChangedEvent,
-com.incquerylabs.smarthome.droolsbundle.TimedDimmer,
-com.incquerylabs.smarthome.eventbusservice.IEventPublisher</t>
-  </si>
-  <si>
     <t>newState == $param</t>
   </si>
   <si>
@@ -193,6 +185,14 @@
 E_Light_Switch_Dimmer_2_Up,
 E_Light_Switch_Dimmer_1_Down,
 E_Light_Switch_Dimmer_2_Down</t>
+  </si>
+  <si>
+    <t>org.eclipse.smarthome.core.items.Item,
+org.eclipse.smarthome.core.library.types.IncreaseDecreaseType,
+org.eclipse.smarthome.core.library.types.OpenClosedType,
+com.incquerylabs.smarthome.eventbusservice.events.ItemStateChangedEvent,
+com.incquerylabs.smarthome.droolsbundle.TimedDimmer,
+com.incquerylabs.smarthome.eventbusservice.IEventPublisher</t>
   </si>
 </sst>
 </file>
@@ -304,12 +304,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -325,6 +319,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -609,7 +609,7 @@
   <dimension ref="A2:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,12 +629,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12" t="s">
-        <v>22</v>
+      <c r="D3" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -649,13 +649,13 @@
       <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>32</v>
+      <c r="D5" s="10" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -686,14 +686,14 @@
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
-      <c r="C11" s="5" t="s">
+      <c r="A11" s="8"/>
+      <c r="C11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="4"/>
+      <c r="E11" s="12"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
@@ -702,7 +702,7 @@
       <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="10"/>
+      <c r="A12" s="8"/>
       <c r="C12" s="2" t="s">
         <v>5</v>
       </c>
@@ -710,7 +710,7 @@
         <v>20</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>15</v>
@@ -722,141 +722,141 @@
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="10"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="8"/>
+      <c r="B13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="9" t="s">
+      <c r="E14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10" t="s">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="9" t="s">
+      <c r="E15" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10" t="s">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="11" t="s">
+      <c r="C17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E16" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F16" s="9" t="s">
+      <c r="E17" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="9" t="s">
+    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
+      <c r="A21" s="8"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="10"/>
+      <c r="A22" s="8"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="10"/>
+      <c r="A23" s="8"/>
       <c r="C23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -868,7 +868,7 @@
       <c r="K23" s="1"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="10"/>
+      <c r="A24" s="8"/>
       <c r="C24" s="2" t="s">
         <v>6</v>
       </c>
@@ -888,14 +888,14 @@
       <c r="K24" s="2"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="10"/>
-      <c r="C25" s="5" t="s">
+      <c r="A25" s="8"/>
+      <c r="C25" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="E25" s="4"/>
+      <c r="E25" s="12"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
@@ -904,7 +904,7 @@
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+      <c r="A26" s="8"/>
       <c r="C26" s="2" t="s">
         <v>5</v>
       </c>
@@ -912,10 +912,10 @@
         <v>20</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -924,67 +924,67 @@
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="8"/>
+      <c r="B27" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="10" t="s">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="11" t="s">
+      <c r="E28" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>29</v>
+      <c r="F28" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>29</v>
+      <c r="E29" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C30" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>29</v>
+      <c r="E30" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactored events on the extended event bus
</commit_message>
<xml_diff>
--- a/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/dtables/dimmer-dtable.xlsx
+++ b/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/dtables/dimmer-dtable.xlsx
@@ -90,9 +90,6 @@
     <t>Variables</t>
   </si>
   <si>
-    <t>newState == $param</t>
-  </si>
-  <si>
     <t>Room A Dimmer Stop</t>
   </si>
   <si>
@@ -193,6 +190,9 @@
   </si>
   <si>
     <t>openhab.timedCommand(TimedDimmer.create($light, $param, 2 , 1000, 50));</t>
+  </si>
+  <si>
+    <t>newState == $param</t>
   </si>
 </sst>
 </file>
@@ -609,16 +609,16 @@
   <dimension ref="A2:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="73.140625" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="71.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -634,7 +634,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -650,12 +650,12 @@
         <v>19</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
@@ -688,7 +688,7 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="C11" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>6</v>
@@ -701,7 +701,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="C12" s="2" t="s">
         <v>4</v>
@@ -710,10 +710,10 @@
         <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F12" s="2" t="s">
         <v>46</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -745,7 +745,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>13</v>
@@ -763,7 +763,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>14</v>
@@ -772,16 +772,16 @@
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
       <c r="B16" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>29</v>
-      </c>
       <c r="E16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>13</v>
@@ -790,16 +790,16 @@
     <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>28</v>
-      </c>
       <c r="D17" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>14</v>
@@ -808,16 +808,16 @@
     <row r="18" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>13</v>
@@ -826,16 +826,16 @@
     <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>36</v>
-      </c>
       <c r="E19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>14</v>
@@ -856,7 +856,7 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="C23" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
@@ -890,7 +890,7 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="C25" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>6</v>
@@ -912,10 +912,10 @@
         <v>18</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
@@ -938,53 +938,53 @@
     <row r="28" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="8"/>
       <c r="B28" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B29" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>32</v>
-      </c>
       <c r="E29" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>39</v>
-      </c>
       <c r="E30" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed TimedCommand to ComplexCommand
</commit_message>
<xml_diff>
--- a/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/dtables/dimmer-dtable.xlsx
+++ b/demo/com.incquerylabs.smarthome.demorules.homeio/src/main/resources/dtables/dimmer-dtable.xlsx
@@ -162,37 +162,37 @@
 E_Light_Switch_Dimmer_2_Down</t>
   </si>
   <si>
+    <t>IEventPublisher openhab,
+IncreaseDecreaseType INCREASE,
+IncreaseDecreaseType DECREASE,
+OpenClosedType PRESSED,
+OpenClosedType RELEASED</t>
+  </si>
+  <si>
+    <t>PRESSED</t>
+  </si>
+  <si>
+    <t>RELEASED</t>
+  </si>
+  <si>
+    <t>$light : Item</t>
+  </si>
+  <si>
+    <t>newState == $param</t>
+  </si>
+  <si>
     <t>org.eclipse.smarthome.core.items.Item,
 org.eclipse.smarthome.core.library.types.IncreaseDecreaseType,
 org.eclipse.smarthome.core.library.types.OpenClosedType,
 com.incquerylabs.smarthome.eventbus.api.events.ItemStateChangedEvent,
 com.incquerylabs.smarthome.eventbus.api.IEventPublisher,
-com.incquerylabs.smarthome.eventbus.ruleengine.droolshomeio.TimedDimmer</t>
-  </si>
-  <si>
-    <t>IEventPublisher openhab,
-IncreaseDecreaseType INCREASE,
-IncreaseDecreaseType DECREASE,
-OpenClosedType PRESSED,
-OpenClosedType RELEASED</t>
-  </si>
-  <si>
-    <t>PRESSED</t>
-  </si>
-  <si>
-    <t>RELEASED</t>
-  </si>
-  <si>
-    <t>$light : Item</t>
-  </si>
-  <si>
-    <t>openhab.stopTimedCommand($light);</t>
-  </si>
-  <si>
-    <t>openhab.timedCommand(TimedDimmer.create($light, $param, 2 , 1000, 50));</t>
-  </si>
-  <si>
-    <t>newState == $param</t>
+com.incquerylabs.smarthome.eventbus.ruleengine.droolshomeio.DimmerCommand</t>
+  </si>
+  <si>
+    <t>openhab.startComplexCommand(DimmerCommand.create($light, $param, 2 , 1000, 50));</t>
+  </si>
+  <si>
+    <t>openhab.stopComplexCommand($light);</t>
   </si>
 </sst>
 </file>
@@ -616,9 +616,9 @@
   <cols>
     <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="4" max="4" width="78.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="70.7109375" customWidth="1"/>
+    <col min="6" max="6" width="70.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -629,12 +629,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -688,7 +688,7 @@
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8"/>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>6</v>
@@ -701,7 +701,7 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="C12" s="2" t="s">
         <v>4</v>
@@ -710,7 +710,7 @@
         <v>18</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>45</v>
@@ -745,7 +745,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F14" s="7" t="s">
         <v>13</v>
@@ -763,7 +763,7 @@
         <v>15</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="7" t="s">
         <v>14</v>
@@ -781,7 +781,7 @@
         <v>28</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>13</v>
@@ -799,7 +799,7 @@
         <v>29</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="7" t="s">
         <v>14</v>
@@ -817,7 +817,7 @@
         <v>36</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F18" s="7" t="s">
         <v>13</v>
@@ -835,7 +835,7 @@
         <v>35</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F19" s="7" t="s">
         <v>14</v>
@@ -890,7 +890,7 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="C25" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D25" s="11" t="s">
         <v>6</v>
@@ -912,7 +912,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F26" s="2" t="s">
         <v>22</v>
@@ -947,10 +947,10 @@
         <v>21</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -964,10 +964,10 @@
         <v>31</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="60" x14ac:dyDescent="0.25">
@@ -981,10 +981,10 @@
         <v>38</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>